<commit_message>
Optimisations et apparition habitants
</commit_message>
<xml_diff>
--- a/Backlogs/MiniTramways-Backlog-16.11.21.xlsx
+++ b/Backlogs/MiniTramways-Backlog-16.11.21.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24706"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24718"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GithubRepos\MiniTramways\Backlogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{631EE117-A8BB-4665-BC8B-38C78702864C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5ADA54A-B11C-45C1-A065-F9F1F5840741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1F765A07-F6B4-4E3C-A596-2A823F0537A9}"/>
+    <workbookView xWindow="2415" yWindow="1110" windowWidth="21600" windowHeight="11295" xr2:uid="{1F765A07-F6B4-4E3C-A596-2A823F0537A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -370,7 +370,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -401,6 +401,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="19">
     <border>
@@ -604,7 +610,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -637,9 +643,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -649,6 +652,8 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -661,8 +666,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -979,8 +988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC90CC32-74CD-4930-AC52-90CD3C0405D5}">
   <dimension ref="A2:V62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1001,22 +1010,22 @@
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="37"/>
-      <c r="D3" s="36" t="s">
+      <c r="C3" s="38"/>
+      <c r="D3" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="37"/>
-      <c r="F3" s="36" t="s">
+      <c r="E3" s="38"/>
+      <c r="F3" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="37"/>
-      <c r="H3" s="36" t="s">
+      <c r="G3" s="38"/>
+      <c r="H3" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="37"/>
+      <c r="I3" s="38"/>
     </row>
     <row r="4" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="26"/>
@@ -1035,16 +1044,16 @@
       </c>
     </row>
     <row r="5" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="33" t="s">
+      <c r="D5" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="E5" s="34" t="s">
+      <c r="E5" s="33" t="s">
         <v>30</v>
       </c>
       <c r="F5" s="18" t="s">
@@ -1061,16 +1070,16 @@
       </c>
     </row>
     <row r="6" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="34" t="s">
         <v>44</v>
       </c>
       <c r="C6" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="D6" s="33" t="s">
+      <c r="D6" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="E6" s="34" t="s">
+      <c r="E6" s="33" t="s">
         <v>37</v>
       </c>
       <c r="F6" s="18" t="s">
@@ -1089,13 +1098,13 @@
     <row r="7" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="25"/>
       <c r="C7" s="19"/>
-      <c r="D7" s="40" t="s">
+      <c r="D7" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="E7" s="41" t="s">
+      <c r="E7" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="29">
+      <c r="F7" s="28">
         <v>1.0131944444444445</v>
       </c>
       <c r="G7" s="19" t="s">
@@ -1111,10 +1120,10 @@
     <row r="8" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="18"/>
       <c r="C8" s="19"/>
-      <c r="D8" s="33" t="s">
+      <c r="D8" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="E8" s="34" t="s">
+      <c r="E8" s="33" t="s">
         <v>89</v>
       </c>
       <c r="F8" s="18" t="s">
@@ -1127,16 +1136,16 @@
       <c r="I8" s="19"/>
     </row>
     <row r="9" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="34" t="s">
+      <c r="C9" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="D9" s="33" t="s">
+      <c r="D9" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="E9" s="34" t="s">
+      <c r="E9" s="33" t="s">
         <v>70</v>
       </c>
       <c r="F9" s="18" t="s">
@@ -1149,16 +1158,16 @@
       <c r="I9" s="19"/>
     </row>
     <row r="10" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="33" t="s">
+      <c r="B10" s="32" t="s">
         <v>97</v>
       </c>
-      <c r="C10" s="34" t="s">
+      <c r="C10" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="D10" s="33" t="s">
+      <c r="D10" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="E10" s="34" t="s">
+      <c r="E10" s="33" t="s">
         <v>72</v>
       </c>
       <c r="F10" s="18" t="s">
@@ -1171,10 +1180,10 @@
       <c r="I10" s="19"/>
     </row>
     <row r="11" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="C11" s="34" t="s">
+      <c r="C11" s="33" t="s">
         <v>83</v>
       </c>
       <c r="F11" s="18" t="s">
@@ -1189,8 +1198,8 @@
     <row r="12" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="18"/>
       <c r="C12" s="19"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="22" t="s">
+      <c r="D12" s="41"/>
+      <c r="E12" s="42" t="s">
         <v>3</v>
       </c>
       <c r="F12" s="18"/>
@@ -1201,10 +1210,10 @@
     <row r="13" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="18"/>
       <c r="C13" s="19"/>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="E13" s="19" t="s">
+      <c r="E13" s="43" t="s">
         <v>75</v>
       </c>
       <c r="F13" s="18"/>
@@ -1215,10 +1224,10 @@
     <row r="14" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="18"/>
       <c r="C14" s="22"/>
-      <c r="D14" s="18" t="s">
+      <c r="D14" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="43" t="s">
         <v>76</v>
       </c>
       <c r="F14" s="18"/>
@@ -1229,10 +1238,10 @@
     <row r="15" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="18"/>
       <c r="C15" s="19"/>
-      <c r="D15" s="28">
+      <c r="D15" s="44">
         <v>17</v>
       </c>
-      <c r="E15" s="19" t="s">
+      <c r="E15" s="43" t="s">
         <v>77</v>
       </c>
       <c r="F15" s="18"/>
@@ -1243,10 +1252,10 @@
     <row r="16" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="18"/>
       <c r="C16" s="19"/>
-      <c r="D16" s="18" t="s">
+      <c r="D16" s="41" t="s">
         <v>98</v>
       </c>
-      <c r="E16" s="19" t="s">
+      <c r="E16" s="43" t="s">
         <v>84</v>
       </c>
       <c r="F16" s="18"/>
@@ -1257,8 +1266,8 @@
     <row r="17" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="18"/>
       <c r="C17" s="19"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="19"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="43"/>
       <c r="F17" s="18"/>
       <c r="G17" s="19"/>
       <c r="H17" s="18"/>
@@ -1267,8 +1276,8 @@
     <row r="18" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="18"/>
       <c r="C18" s="19"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="22" t="s">
+      <c r="D18" s="41"/>
+      <c r="E18" s="42" t="s">
         <v>4</v>
       </c>
       <c r="F18" s="18"/>
@@ -1279,10 +1288,10 @@
     <row r="19" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="18"/>
       <c r="C19" s="19"/>
-      <c r="D19" s="18" t="s">
+      <c r="D19" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="E19" s="19" t="s">
+      <c r="E19" s="43" t="s">
         <v>31</v>
       </c>
       <c r="F19" s="18"/>
@@ -1293,10 +1302,10 @@
     <row r="20" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="18"/>
       <c r="C20" s="19"/>
-      <c r="D20" s="18" t="s">
+      <c r="D20" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="E20" s="19" t="s">
+      <c r="E20" s="43" t="s">
         <v>79</v>
       </c>
       <c r="F20" s="18"/>
@@ -1306,10 +1315,10 @@
     </row>
     <row r="21" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="23"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="32"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="31"/>
       <c r="E21" s="24"/>
-      <c r="F21" s="31"/>
+      <c r="F21" s="30"/>
       <c r="G21" s="24"/>
       <c r="H21" s="23"/>
       <c r="I21" s="24"/>
@@ -1326,18 +1335,18 @@
       <c r="A27" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="38" t="s">
+      <c r="B27" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C27" s="39"/>
-      <c r="D27" s="38" t="s">
+      <c r="C27" s="40"/>
+      <c r="D27" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="E27" s="39"/>
-      <c r="F27" s="38" t="s">
+      <c r="E27" s="40"/>
+      <c r="F27" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="G27" s="39"/>
+      <c r="G27" s="40"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B28" s="5"/>
@@ -1417,18 +1426,18 @@
       <c r="A37" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B37" s="38" t="s">
+      <c r="B37" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C37" s="39"/>
-      <c r="D37" s="38" t="s">
+      <c r="C37" s="40"/>
+      <c r="D37" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="E37" s="39"/>
-      <c r="F37" s="38" t="s">
+      <c r="E37" s="40"/>
+      <c r="F37" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="G37" s="39"/>
+      <c r="G37" s="40"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B38" s="13"/>

</xml_diff>